<commit_message>
added first five questions solutions
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1844,7 +1844,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1855,7 +1855,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1921,7 +1921,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21">
@@ -1932,7 +1932,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21">
@@ -1943,7 +1943,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21">

</xml_diff>